<commit_message>
excel file upload to database successfully
</commit_message>
<xml_diff>
--- a/ExcelFiles/CapitalgaincalculationTestingcandidate.xlsx
+++ b/ExcelFiles/CapitalgaincalculationTestingcandidate.xlsx
@@ -9,11 +9,9 @@
   <sheets>
     <sheet name="Transaction_with_corporate_acti" sheetId="7" r:id="rId1"/>
     <sheet name="Calculation sheet" sheetId="10" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="11" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Transaction_with_corporate_acti!$A$2:$G$2</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -60,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="39">
   <si>
     <t>Asset Name</t>
   </si>
@@ -175,6 +173,9 @@
   <si>
     <t>BLUESTAR</t>
   </si>
+  <si>
+    <t>how to delete drawing shape in excel</t>
+  </si>
 </sst>
 </file>
 
@@ -186,7 +187,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,6 +230,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFECECF1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -318,7 +325,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -441,6 +448,7 @@
     <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -482,188 +490,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="3238500" cy="2675732"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AD0EE308-617D-445C-B39C-8D993C687C96}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6257925" y="885824"/>
-          <a:ext cx="3238500" cy="2675732"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Step</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> 1 </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>This transcation will be coming as</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> a excel sheet and will be uploaded to the software </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" baseline="0">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Step 2</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" baseline="0">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>After uploading this excel file, system will calculate capital gain with various conditions mentioned in calculation sheet </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" baseline="0">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> Step 3</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100" baseline="0">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Show total value of long term capital gain (LTCG)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -953,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,7 +797,7 @@
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>4</v>
       </c>
@@ -993,19 +819,37 @@
       <c r="G1" s="35" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="35"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1"/>
+      <c r="I1"/>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="39">
+        <v>43979</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="30">
+        <v>100</v>
+      </c>
+      <c r="E2" s="31">
+        <v>339.88150000000002</v>
+      </c>
+      <c r="F2" s="31">
+        <v>33988.15</v>
+      </c>
+      <c r="G2" s="36">
+        <v>100</v>
+      </c>
+      <c r="H2"/>
+      <c r="I2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="39">
-        <v>43979</v>
+        <v>43980</v>
       </c>
       <c r="B3" s="30" t="s">
         <v>9</v>
@@ -1017,18 +861,18 @@
         <v>100</v>
       </c>
       <c r="E3" s="31">
-        <v>339.88150000000002</v>
+        <v>342.61509999999998</v>
       </c>
       <c r="F3" s="31">
-        <v>33988.15</v>
+        <v>34261.51</v>
       </c>
       <c r="G3" s="36">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="39">
-        <v>43980</v>
+        <v>43984</v>
       </c>
       <c r="B4" s="30" t="s">
         <v>9</v>
@@ -1040,21 +884,21 @@
         <v>100</v>
       </c>
       <c r="E4" s="31">
-        <v>342.61509999999998</v>
+        <v>355.97</v>
       </c>
       <c r="F4" s="31">
-        <v>34261.51</v>
+        <v>35597</v>
       </c>
       <c r="G4" s="36">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="39">
-        <v>43984</v>
+        <v>43992</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C5" s="30" t="s">
         <v>13</v>
@@ -1063,18 +907,18 @@
         <v>100</v>
       </c>
       <c r="E5" s="31">
-        <v>355.97</v>
+        <v>400.98</v>
       </c>
       <c r="F5" s="31">
-        <v>35597</v>
+        <v>40098</v>
       </c>
       <c r="G5" s="36">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="39">
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="B6" s="30" t="s">
         <v>12</v>
@@ -1086,18 +930,18 @@
         <v>100</v>
       </c>
       <c r="E6" s="31">
-        <v>400.98</v>
+        <v>386.46</v>
       </c>
       <c r="F6" s="31">
-        <v>40098</v>
+        <v>38646</v>
       </c>
       <c r="G6" s="36">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="39">
-        <v>43993</v>
+        <v>43997</v>
       </c>
       <c r="B7" s="30" t="s">
         <v>12</v>
@@ -1109,105 +953,133 @@
         <v>100</v>
       </c>
       <c r="E7" s="31">
-        <v>386.46</v>
+        <v>389.29</v>
       </c>
       <c r="F7" s="31">
-        <v>38646</v>
+        <v>38929</v>
       </c>
       <c r="G7" s="36">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="39">
-        <v>43997</v>
+        <v>43966</v>
       </c>
       <c r="B8" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="30">
+        <v>50</v>
+      </c>
+      <c r="E8" s="31">
+        <v>1531.72</v>
+      </c>
+      <c r="F8" s="31">
+        <v>76586</v>
+      </c>
+      <c r="G8" s="36">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="39">
+        <v>43977</v>
+      </c>
+      <c r="B9" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="30">
-        <v>100</v>
-      </c>
-      <c r="E8" s="31">
-        <v>389.29</v>
-      </c>
-      <c r="F8" s="31">
-        <v>38929</v>
-      </c>
-      <c r="G8" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="39"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="36"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="30">
+        <v>50</v>
+      </c>
+      <c r="E9" s="31">
+        <v>1627.17</v>
+      </c>
+      <c r="F9" s="31">
+        <v>81358.5</v>
+      </c>
+      <c r="G9" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="39">
-        <v>43966</v>
+        <v>43992</v>
       </c>
       <c r="B10" s="30" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D10" s="30">
+        <v>150</v>
+      </c>
+      <c r="E10" s="31">
+        <v>570.94000000000005</v>
+      </c>
+      <c r="F10" s="31">
+        <v>85641</v>
+      </c>
+      <c r="G10" s="36">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="39">
+        <v>43994</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="30">
+        <v>200</v>
+      </c>
+      <c r="E11" s="31">
+        <v>562.5</v>
+      </c>
+      <c r="F11" s="31">
+        <v>112500</v>
+      </c>
+      <c r="G11" s="36">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="39">
+        <v>44035</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="30">
         <v>50</v>
       </c>
-      <c r="E10" s="31">
-        <v>1531.72</v>
-      </c>
-      <c r="F10" s="31">
-        <v>76586</v>
-      </c>
-      <c r="G10" s="36">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="39">
-        <v>43977</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="30">
-        <v>50</v>
-      </c>
-      <c r="E11" s="31">
-        <v>1627.17</v>
-      </c>
-      <c r="F11" s="31">
-        <v>81358.5</v>
-      </c>
-      <c r="G11" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="36"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E12" s="31">
+        <v>572.6</v>
+      </c>
+      <c r="F12" s="31">
+        <v>28630</v>
+      </c>
+      <c r="G12" s="36">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="39">
-        <v>43992</v>
+        <v>44092</v>
       </c>
       <c r="B13" s="30" t="s">
         <v>9</v>
@@ -1216,122 +1088,136 @@
         <v>14</v>
       </c>
       <c r="D13" s="30">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E13" s="31">
-        <v>570.94000000000005</v>
+        <v>492.5</v>
       </c>
       <c r="F13" s="31">
-        <v>85641</v>
+        <v>49250</v>
       </c>
       <c r="G13" s="36">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="39">
-        <v>43994</v>
+        <v>44097</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C14" s="30" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="30">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="E14" s="31">
-        <v>562.5</v>
+        <v>430.59649999999999</v>
       </c>
       <c r="F14" s="31">
-        <v>112500</v>
+        <v>215298.25</v>
       </c>
       <c r="G14" s="36">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="39">
-        <v>44035</v>
+        <v>42862</v>
       </c>
       <c r="B15" s="30" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D15" s="30">
         <v>50</v>
       </c>
       <c r="E15" s="31">
-        <v>572.6</v>
+        <v>679</v>
       </c>
       <c r="F15" s="31">
-        <v>28630</v>
+        <v>40180.43</v>
       </c>
       <c r="G15" s="36">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="39">
-        <v>44092</v>
+        <v>43241</v>
       </c>
       <c r="B16" s="30" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D16" s="30">
+        <v>50</v>
+      </c>
+      <c r="E16" s="31">
+        <v>710.54</v>
+      </c>
+      <c r="F16" s="31">
+        <v>35527</v>
+      </c>
+      <c r="G16" s="36">
         <v>100</v>
       </c>
-      <c r="E16" s="31">
-        <v>492.5</v>
-      </c>
-      <c r="F16" s="31">
-        <v>49250</v>
-      </c>
-      <c r="G16" s="36">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="39">
-        <v>44097</v>
+        <v>43245</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D17" s="30">
-        <v>500</v>
+        <v>20</v>
       </c>
       <c r="E17" s="31">
-        <v>430.59649999999999</v>
+        <v>701.69</v>
       </c>
       <c r="F17" s="31">
-        <v>215298.25</v>
+        <v>14033.8</v>
       </c>
       <c r="G17" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="39"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="36"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="39">
+        <v>43258</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="30">
+        <v>30</v>
+      </c>
+      <c r="E18" s="31">
+        <v>677.97</v>
+      </c>
+      <c r="F18" s="31">
+        <v>20339.099999999999</v>
+      </c>
+      <c r="G18" s="36">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="39">
-        <v>42862</v>
+        <v>43280</v>
       </c>
       <c r="B19" s="30" t="s">
         <v>9</v>
@@ -1343,18 +1229,18 @@
         <v>50</v>
       </c>
       <c r="E19" s="31">
-        <v>679</v>
+        <v>649.13</v>
       </c>
       <c r="F19" s="31">
-        <v>40180.43</v>
+        <v>32456.5</v>
       </c>
       <c r="G19" s="36">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="39">
-        <v>43241</v>
+        <v>43304</v>
       </c>
       <c r="B20" s="30" t="s">
         <v>9</v>
@@ -1366,18 +1252,18 @@
         <v>50</v>
       </c>
       <c r="E20" s="31">
-        <v>710.54</v>
+        <v>676.34119999999996</v>
       </c>
       <c r="F20" s="31">
-        <v>35527</v>
+        <v>33817.06</v>
       </c>
       <c r="G20" s="36">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="39">
-        <v>43245</v>
+        <v>43362</v>
       </c>
       <c r="B21" s="30" t="s">
         <v>9</v>
@@ -1386,160 +1272,159 @@
         <v>10</v>
       </c>
       <c r="D21" s="30">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E21" s="31">
-        <v>701.69</v>
+        <v>660.44</v>
       </c>
       <c r="F21" s="31">
-        <v>14033.8</v>
+        <v>33022</v>
       </c>
       <c r="G21" s="36">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="39">
-        <v>43258</v>
+        <v>43924</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C22" s="30" t="s">
         <v>10</v>
       </c>
       <c r="D22" s="30">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="E22" s="31">
-        <v>677.97</v>
+        <v>449.59890000000001</v>
       </c>
       <c r="F22" s="31">
-        <v>20339.099999999999</v>
+        <v>134879.67000000001</v>
       </c>
       <c r="G22" s="36">
-        <v>150</v>
-      </c>
-      <c r="J22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="39">
-        <v>43280</v>
+        <v>43831</v>
       </c>
       <c r="B23" s="30" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D23" s="30">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="E23" s="31">
-        <v>649.13</v>
+        <v>224.87</v>
       </c>
       <c r="F23" s="31">
-        <v>32456.5</v>
+        <v>44974</v>
       </c>
       <c r="G23" s="36">
         <v>200</v>
       </c>
-      <c r="J23" t="s">
-        <v>11</v>
-      </c>
-      <c r="K23">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="39">
-        <v>43304</v>
+        <v>43840</v>
       </c>
       <c r="B24" s="30" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D24" s="30">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="E24" s="31">
-        <v>676.34119999999996</v>
+        <v>259.64</v>
       </c>
       <c r="F24" s="31">
-        <v>33817.06</v>
+        <v>51928</v>
       </c>
       <c r="G24" s="36">
-        <v>250</v>
-      </c>
-      <c r="J24" t="s">
-        <v>37</v>
-      </c>
-      <c r="K24">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="39">
-        <v>43362</v>
+        <v>43864</v>
       </c>
       <c r="B25" s="30" t="s">
         <v>9</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D25" s="30">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E25" s="31">
-        <v>660.44</v>
+        <v>256.38</v>
       </c>
       <c r="F25" s="31">
-        <v>33022</v>
+        <v>25638</v>
       </c>
       <c r="G25" s="36">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="39">
-        <v>43924</v>
+        <v>43892</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D26" s="30">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="E26" s="31">
-        <v>449.59890000000001</v>
+        <v>269.49</v>
       </c>
       <c r="F26" s="31">
-        <v>134879.67000000001</v>
+        <v>26949</v>
       </c>
       <c r="G26" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="39"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="36"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="39">
+        <v>43899</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="30">
+        <v>200</v>
+      </c>
+      <c r="E27" s="31">
+        <v>242.36</v>
+      </c>
+      <c r="F27" s="31">
+        <v>48472</v>
+      </c>
+      <c r="G27" s="36">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="39">
-        <v>43831</v>
+        <v>44028</v>
       </c>
       <c r="B28" s="30" t="s">
         <v>9</v>
@@ -1551,21 +1436,21 @@
         <v>200</v>
       </c>
       <c r="E28" s="31">
-        <v>224.87</v>
+        <v>290.44369999999998</v>
       </c>
       <c r="F28" s="31">
-        <v>44974</v>
+        <v>58088.74</v>
       </c>
       <c r="G28" s="36">
         <v>200</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="39">
-        <v>43840</v>
+        <v>44036</v>
       </c>
       <c r="B29" s="30" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C29" s="30" t="s">
         <v>3</v>
@@ -1574,62 +1459,62 @@
         <v>200</v>
       </c>
       <c r="E29" s="31">
-        <v>259.64</v>
+        <v>318.05</v>
       </c>
       <c r="F29" s="31">
-        <v>51928</v>
+        <v>63610</v>
       </c>
       <c r="G29" s="36">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="39">
-        <v>43864</v>
+        <v>43046</v>
       </c>
       <c r="B30" s="30" t="s">
         <v>9</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D30" s="30">
         <v>100</v>
       </c>
       <c r="E30" s="31">
-        <v>256.38</v>
+        <v>250</v>
       </c>
       <c r="F30" s="31">
-        <v>25638</v>
+        <v>30375.1</v>
       </c>
       <c r="G30" s="36">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="39">
-        <v>43892</v>
+        <v>43777</v>
       </c>
       <c r="B31" s="30" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="30" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D31" s="30">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="E31" s="31">
-        <v>269.49</v>
+        <v>300.5</v>
       </c>
       <c r="F31" s="31">
-        <v>26949</v>
+        <v>90150</v>
       </c>
       <c r="G31" s="36">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="39">
         <v>43899</v>
       </c>
@@ -1637,252 +1522,114 @@
         <v>9</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D32" s="30">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="E32" s="31">
-        <v>242.36</v>
+        <v>275.06950000000001</v>
       </c>
       <c r="F32" s="31">
-        <v>48472</v>
+        <v>27506.95</v>
       </c>
       <c r="G32" s="36">
-        <v>800</v>
+        <v>500</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="39">
-        <v>44028</v>
+        <v>43955</v>
       </c>
       <c r="B33" s="30" t="s">
         <v>9</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="D33" s="30">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="E33" s="31">
-        <v>290.44369999999998</v>
+        <v>145.66999999999999</v>
       </c>
       <c r="F33" s="31">
-        <v>58088.74</v>
+        <v>58268</v>
       </c>
       <c r="G33" s="36">
-        <v>200</v>
+        <v>900</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="39">
-        <v>44036</v>
+        <v>43978</v>
       </c>
       <c r="B34" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="30">
+        <v>100</v>
+      </c>
+      <c r="E34" s="31">
+        <v>129.80000000000001</v>
+      </c>
+      <c r="F34" s="31">
+        <v>12980</v>
+      </c>
+      <c r="G34" s="36">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="39">
+        <v>43999</v>
+      </c>
+      <c r="B35" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="D34" s="30">
-        <v>200</v>
-      </c>
-      <c r="E34" s="31">
-        <v>318.05</v>
-      </c>
-      <c r="F34" s="31">
-        <v>63610</v>
-      </c>
-      <c r="G34" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="39"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="36"/>
+      <c r="C35" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="30">
+        <v>500</v>
+      </c>
+      <c r="E35" s="31">
+        <v>166.66499999999999</v>
+      </c>
+      <c r="F35" s="31">
+        <v>83332.5</v>
+      </c>
+      <c r="G35" s="36">
+        <v>500</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="39">
-        <v>43046</v>
+        <v>44130</v>
       </c>
       <c r="B36" s="30" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C36" s="30" t="s">
         <v>11</v>
       </c>
       <c r="D36" s="30">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="E36" s="31">
-        <v>250</v>
+        <v>247.9</v>
       </c>
       <c r="F36" s="31">
-        <v>30375.1</v>
+        <v>123950</v>
       </c>
       <c r="G36" s="36">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="39">
-        <v>43777</v>
-      </c>
-      <c r="B37" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="30">
-        <v>300</v>
-      </c>
-      <c r="E37" s="31">
-        <v>300.5</v>
-      </c>
-      <c r="F37" s="31">
-        <v>90150</v>
-      </c>
-      <c r="G37" s="36">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="39">
-        <v>43899</v>
-      </c>
-      <c r="B38" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" s="30">
-        <v>100</v>
-      </c>
-      <c r="E38" s="31">
-        <v>275.06950000000001</v>
-      </c>
-      <c r="F38" s="31">
-        <v>27506.95</v>
-      </c>
-      <c r="G38" s="36">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="39">
-        <v>43955</v>
-      </c>
-      <c r="B39" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="30">
-        <v>400</v>
-      </c>
-      <c r="E39" s="31">
-        <v>145.66999999999999</v>
-      </c>
-      <c r="F39" s="31">
-        <v>58268</v>
-      </c>
-      <c r="G39" s="36">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="39">
-        <v>43978</v>
-      </c>
-      <c r="B40" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="D40" s="30">
-        <v>100</v>
-      </c>
-      <c r="E40" s="31">
-        <v>129.80000000000001</v>
-      </c>
-      <c r="F40" s="31">
-        <v>12980</v>
-      </c>
-      <c r="G40" s="36">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="39">
-        <v>43999</v>
-      </c>
-      <c r="B41" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="C41" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="D41" s="30">
-        <v>500</v>
-      </c>
-      <c r="E41" s="31">
-        <v>166.66499999999999</v>
-      </c>
-      <c r="F41" s="31">
-        <v>83332.5</v>
-      </c>
-      <c r="G41" s="36">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="39">
-        <v>44130</v>
-      </c>
-      <c r="B42" s="30" t="s">
-        <v>12</v>
-      </c>
-      <c r="C42" s="30" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" s="30">
-        <v>500</v>
-      </c>
-      <c r="E42" s="31">
-        <v>247.9</v>
-      </c>
-      <c r="F42" s="31">
-        <v>123950</v>
-      </c>
-      <c r="G42" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="39"/>
-      <c r="B43" s="30"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="36"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:G2">
-    <sortState ref="A3:G43">
-      <sortCondition ref="C2"/>
-    </sortState>
-  </autoFilter>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="SPLIT">
       <formula>NOT(ISERROR(SEARCH("SPLIT",B1)))</formula>
@@ -1896,7 +1643,6 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -12686,4 +12432,46 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="F5" s="42" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>